<commit_message>
updates to final results
</commit_message>
<xml_diff>
--- a/data/growth habits guide.xlsx
+++ b/data/growth habits guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Australian-plant-photos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69BBE43-A40F-44B0-95AA-914F5D987166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6B5ED9-428D-4454-A0AC-8595E88234CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{61B491D9-5703-4DC7-8FB0-B07B7908227B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
   <si>
     <t>shrub</t>
   </si>
@@ -178,9 +178,6 @@
     <t>climber_shrub</t>
   </si>
   <si>
-    <t>climber_liana tree</t>
-  </si>
-  <si>
     <t>original</t>
   </si>
   <si>
@@ -413,6 +410,9 @@
   </si>
   <si>
     <t>fern (tree, terres, litho)</t>
+  </si>
+  <si>
+    <t>original number</t>
   </si>
 </sst>
 </file>
@@ -764,7 +764,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F293D1A1-B228-43E0-B612-9427AD834331}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
@@ -772,403 +772,546 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1281</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>B16+B19+B22+B23+B29</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>431</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="B44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="B45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="B46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="B47" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
-      <c r="B48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" t="s">
-        <v>52</v>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C48">
+    <sortCondition descending="1" ref="B2:B48"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1178,7 +1321,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B4" sqref="B4:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,151 +1332,151 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1341,7 +1484,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1349,7 +1492,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1357,7 +1500,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1365,7 +1508,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -1373,23 +1516,23 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -1397,15 +1540,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1413,23 +1556,23 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -1437,7 +1580,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -1445,7 +1588,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -1453,7 +1596,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -1461,7 +1604,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -1469,7 +1612,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -1477,7 +1620,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -1485,7 +1628,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -1493,7 +1636,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -1501,7 +1644,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -1509,7 +1652,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -1517,7 +1660,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -1525,7 +1668,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -1533,7 +1676,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -1541,7 +1684,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
@@ -1549,7 +1692,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -1557,7 +1700,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -1565,7 +1708,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -1573,7 +1716,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
@@ -1581,29 +1724,32 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B52">
+    <sortCondition ref="B2:B52"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1614,7 +1760,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,15 +1771,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1641,15 +1787,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1657,7 +1803,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1665,7 +1811,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1673,23 +1819,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -1697,7 +1843,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -1705,7 +1851,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -1713,7 +1859,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1721,7 +1867,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1729,7 +1875,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1745,7 +1891,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,10 +1901,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1766,7 +1912,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1431</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1774,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1308</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1782,7 +1928,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1790,44 +1936,44 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="B7">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="B8">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <v>13</v>
@@ -1835,7 +1981,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1843,7 +1989,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12">
         <v>1</v>

</xml_diff>

<commit_message>
updates to main apc file
</commit_message>
<xml_diff>
--- a/data/growth habits guide.xlsx
+++ b/data/growth habits guide.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Australian-plant-photos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8038E74D-2BEB-49EA-AB25-08261ED037A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D5911D-C3C3-4C01-95DD-02F2E00FA6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{61B491D9-5703-4DC7-8FB0-B07B7908227B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{61B491D9-5703-4DC7-8FB0-B07B7908227B}"/>
   </bookViews>
   <sheets>
-    <sheet name="replacements" sheetId="1" r:id="rId1"/>
-    <sheet name="fern" sheetId="2" r:id="rId2"/>
-    <sheet name="unscored" sheetId="3" r:id="rId3"/>
-    <sheet name="final counts" sheetId="4" r:id="rId4"/>
+    <sheet name="replacements (unphotographed)" sheetId="1" r:id="rId1"/>
+    <sheet name="ferns (unphotographed)" sheetId="2" r:id="rId2"/>
+    <sheet name="unscored (unphotographed)" sheetId="3" r:id="rId3"/>
+    <sheet name="final counts (unphotographed)" sheetId="4" r:id="rId4"/>
+    <sheet name="replacements (all species)" sheetId="5" r:id="rId5"/>
+    <sheet name="ferns (all species)" sheetId="6" r:id="rId6"/>
+    <sheet name="unscored (all species)" sheetId="7" r:id="rId7"/>
+    <sheet name="final counts (all species)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="125">
   <si>
     <t>shrub</t>
   </si>
@@ -428,18 +432,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -454,9 +452,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -774,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F293D1A1-B228-43E0-B612-9427AD834331}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +870,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -895,7 +892,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -906,7 +903,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B12">
@@ -917,7 +914,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13">
@@ -928,7 +925,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14">
@@ -950,7 +947,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16">
@@ -1325,7 +1322,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,7 +1761,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A3:B16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,108 +1787,108 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1903,7 +1900,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,4 +2010,1240 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE00787-7542-425F-B3EC-9EFCE3B59953}">
+  <dimension ref="A1:C48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1280</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>431</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62329DFF-86E4-48DA-B25C-A0AAC4761D4C}">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC27D81B-81E2-4F34-A871-C86CA82E872C}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB6B8DE-FE85-4D1F-A7B9-465EEAC24C84}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>